<commit_message>
create a scratch file
</commit_message>
<xml_diff>
--- a/regression_hdi/hdi_2015.xlsx
+++ b/regression_hdi/hdi_2015.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\03_research_and_development\01_research_topics\paper_0_CRD_main\lesson_plans\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\03_research_and_development\01_research_topics\paper_0_CRD_main\lesson_plans\crd_paper_lessons\regression_hdi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE20918D-6736-4F50-A803-8AE73DC7B561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB68EA9-B087-4A7E-B160-D66127BD759B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="1260" windowWidth="17250" windowHeight="8910" activeTab="1" xr2:uid="{168A8524-24AB-42D7-BE2E-5974113DED0B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{168A8524-24AB-42D7-BE2E-5974113DED0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="243">
   <si>
     <t>Country</t>
   </si>
@@ -689,6 +689,81 @@
   </si>
   <si>
     <t>natural_order</t>
+  </si>
+  <si>
+    <t>abbreviations</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>HDI_Rank</t>
+  </si>
+  <si>
+    <t>Life_expectancy_at_birth</t>
+  </si>
+  <si>
+    <t>Expected_years_of_schooling</t>
+  </si>
+  <si>
+    <t>Mean_years_of_schooling</t>
+  </si>
+  <si>
+    <t>HDI_rank2</t>
+  </si>
+  <si>
+    <t>Fertility_Rate</t>
+  </si>
+  <si>
+    <t>Human_Development_Index_HDI</t>
+  </si>
+  <si>
+    <t>Population_millions</t>
+  </si>
+  <si>
+    <t>Est_Population_2030_millions</t>
+  </si>
+  <si>
+    <t>Gross_national_income_GNI_per_capita</t>
+  </si>
+  <si>
+    <t>Net_Migration_per_1000</t>
+  </si>
+  <si>
+    <t>Tourists_000s</t>
+  </si>
+  <si>
+    <t>Mobile_Phone_per_100</t>
+  </si>
+  <si>
+    <t>Under_age_5_millions</t>
+  </si>
+  <si>
+    <t>Median_age_years</t>
+  </si>
+  <si>
+    <t>Young_0_14_per_100_adults_15_64</t>
+  </si>
+  <si>
+    <t>Old_65_and_olderper_100_adults_15_64</t>
+  </si>
+  <si>
+    <t>Sex_ratio_at_birth_male_to_female_births</t>
+  </si>
+  <si>
+    <t>Trade_Percent_GDP</t>
+  </si>
+  <si>
+    <t>Foreign_Investment_Percent_GDP</t>
+  </si>
+  <si>
+    <t>Internet_Users_Percent</t>
+  </si>
+  <si>
+    <t>Avg_Annual_Growth_Percent</t>
+  </si>
+  <si>
+    <t>Urban_Percent</t>
   </si>
 </sst>
 </file>
@@ -704,7 +779,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -719,7 +793,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -728,45 +802,241 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
+        <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -784,21 +1054,121 @@
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
-        <right/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
+          <color indexed="64"/>
         </top>
         <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
+          <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -850,17 +1220,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5D15054F-9A9D-44CD-865A-436B604321D7}" name="Table2" displayName="Table2" ref="A1:C24" totalsRowShown="0">
-  <autoFilter ref="A1:C24" xr:uid="{5D15054F-9A9D-44CD-865A-436B604321D7}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C24">
-    <sortCondition ref="B1:B24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5D15054F-9A9D-44CD-865A-436B604321D7}" name="Table2" displayName="Table2" ref="A1:D25" totalsRowShown="0" headerRowDxfId="0" dataDxfId="8" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
+  <autoFilter ref="A1:D25" xr:uid="{5D15054F-9A9D-44CD-865A-436B604321D7}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D25">
+    <sortCondition ref="D1:D25"/>
   </sortState>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{615CA706-1C27-4D6E-8852-51BCA6C3DA77}" name="Variable" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{8A56FE7B-B88A-4806-B0B9-FF5DD5CF55AA}" name="Variable Classification"/>
-    <tableColumn id="3" xr3:uid="{7D7A9526-B514-4569-8D17-95D09ADB7389}" name="natural_order"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{615CA706-1C27-4D6E-8852-51BCA6C3DA77}" name="Variable" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{47BD8A9E-F228-48BA-AD21-28F8CA491246}" name="abbreviations" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{8A56FE7B-B88A-4806-B0B9-FF5DD5CF55AA}" name="Variable Classification" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{7D7A9526-B514-4569-8D17-95D09ADB7389}" name="natural_order" dataDxfId="1"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1163,9 +1534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7B3615F-7964-4D32-A076-5A7784B9B9BC}">
   <dimension ref="A1:X189"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V7" sqref="V7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -15020,268 +15389,362 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47D96A8B-A39C-422D-8CEA-D7BC35326996}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="155" zoomScaleNormal="155" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" customWidth="1"/>
-    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="1" max="2" width="41.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="4" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D5" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D6" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D7" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B8" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="C2">
+      <c r="D8" s="7">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B9" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="C3">
+      <c r="D9" s="7">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="D10" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="D11" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="D12" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="D14" s="7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="D15" s="7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="D16" s="7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="D18" s="7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="D19" s="7">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="D20" s="7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="D21" s="7">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="C7">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="D22" s="7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="C8">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="D23" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="C9">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="D24" s="7">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="C10">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>212</v>
-      </c>
-      <c r="C11">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" t="s">
-        <v>212</v>
-      </c>
-      <c r="C12">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" t="s">
-        <v>212</v>
-      </c>
-      <c r="C13">
+      <c r="D25" s="10">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" t="s">
-        <v>213</v>
-      </c>
-      <c r="C14">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" t="s">
-        <v>213</v>
-      </c>
-      <c r="C15">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" t="s">
-        <v>213</v>
-      </c>
-      <c r="C16">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" t="s">
-        <v>213</v>
-      </c>
-      <c r="C17">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" t="s">
-        <v>213</v>
-      </c>
-      <c r="C18">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" t="s">
-        <v>213</v>
-      </c>
-      <c r="C19">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" t="s">
-        <v>213</v>
-      </c>
-      <c r="C20">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C24">
-        <v>15</v>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made major changes to app
</commit_message>
<xml_diff>
--- a/regression_hdi/hdi_2015.xlsx
+++ b/regression_hdi/hdi_2015.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\03_research_and_development\01_research_topics\paper_0_CRD_main\lesson_plans\crd_paper_lessons\regression_hdi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB68EA9-B087-4A7E-B160-D66127BD759B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED1E992-20CC-4006-9F47-15754A6F7C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{168A8524-24AB-42D7-BE2E-5974113DED0B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="raw_data" sheetId="2" r:id="rId1"/>
+    <sheet name="variables" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -694,9 +694,6 @@
     <t>abbreviations</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>HDI_Rank</t>
   </si>
   <si>
@@ -764,6 +761,9 @@
   </si>
   <si>
     <t>Urban_Percent</t>
+  </si>
+  <si>
+    <t>ignore_variables</t>
   </si>
 </sst>
 </file>
@@ -916,7 +916,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -928,33 +928,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
     <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1128,13 +1126,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1169,6 +1160,36 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1220,16 +1241,17 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5D15054F-9A9D-44CD-865A-436B604321D7}" name="Table2" displayName="Table2" ref="A1:D25" totalsRowShown="0" headerRowDxfId="0" dataDxfId="8" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
-  <autoFilter ref="A1:D25" xr:uid="{5D15054F-9A9D-44CD-865A-436B604321D7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5D15054F-9A9D-44CD-865A-436B604321D7}" name="Table2" displayName="Table2" ref="A1:E25" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+  <autoFilter ref="A1:E25" xr:uid="{5D15054F-9A9D-44CD-865A-436B604321D7}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D25">
     <sortCondition ref="D1:D25"/>
   </sortState>
-  <tableColumns count="4">
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{615CA706-1C27-4D6E-8852-51BCA6C3DA77}" name="Variable" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{47BD8A9E-F228-48BA-AD21-28F8CA491246}" name="abbreviations" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{8A56FE7B-B88A-4806-B0B9-FF5DD5CF55AA}" name="Variable Classification" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{7D7A9526-B514-4569-8D17-95D09ADB7389}" name="natural_order" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{32CE4449-EABA-4D37-A914-4FBD2F8D6D7C}" name="ignore_variables" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1534,7 +1556,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7B3615F-7964-4D32-A076-5A7784B9B9BC}">
   <dimension ref="A1:X189"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -15389,10 +15413,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47D96A8B-A39C-422D-8CEA-D7BC35326996}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="155" zoomScaleNormal="155" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15402,7 +15426,7 @@
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>215</v>
       </c>
@@ -15415,8 +15439,11 @@
       <c r="D1" s="4" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -15427,37 +15454,46 @@
       <c r="D2" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>212</v>
@@ -15465,13 +15501,14 @@
       <c r="D5" s="7">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="11"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>212</v>
@@ -15479,13 +15516,14 @@
       <c r="D6" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="11"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>212</v>
@@ -15493,13 +15531,14 @@
       <c r="D7" s="7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="11"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>214</v>
@@ -15507,13 +15546,14 @@
       <c r="D8" s="7">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>214</v>
@@ -15521,13 +15561,14 @@
       <c r="D9" s="7">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="11"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>213</v>
@@ -15535,13 +15576,14 @@
       <c r="D10" s="7">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="11"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>213</v>
@@ -15549,13 +15591,14 @@
       <c r="D11" s="7">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="11"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>213</v>
@@ -15563,25 +15606,27 @@
       <c r="D12" s="7">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="11"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="7">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="11"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>213</v>
@@ -15589,13 +15634,14 @@
       <c r="D14" s="7">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="11"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>213</v>
@@ -15603,13 +15649,14 @@
       <c r="D15" s="7">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="11"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>213</v>
@@ -15617,25 +15664,29 @@
       <c r="D16" s="7">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="11"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>211</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="7">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>212</v>
@@ -15643,13 +15694,14 @@
       <c r="D18" s="7">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="11"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>213</v>
@@ -15657,13 +15709,14 @@
       <c r="D19" s="7">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="11"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>212</v>
@@ -15671,13 +15724,14 @@
       <c r="D20" s="7">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="11"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>212</v>
@@ -15685,13 +15739,14 @@
       <c r="D21" s="7">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="11"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>212</v>
@@ -15699,13 +15754,14 @@
       <c r="D22" s="7">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="11"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>212</v>
@@ -15713,13 +15769,14 @@
       <c r="D23" s="7">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="11"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>212</v>
@@ -15727,13 +15784,14 @@
       <c r="D24" s="7">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="11"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>212</v>
@@ -15741,11 +15799,7 @@
       <c r="D25" s="10">
         <v>23</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
-        <v>219</v>
-      </c>
+      <c r="E25" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>